<commit_message>
channel gtc and validation importrow plandc
</commit_message>
<xml_diff>
--- a/public/assets/EmployeeDcImport.xlsx
+++ b/public/assets/EmployeeDcImport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="8535"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9630"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>NIK</t>
   </si>
@@ -64,6 +64,36 @@
   </si>
   <si>
     <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>fafaf</t>
+  </si>
+  <si>
+    <t>gg</t>
+  </si>
+  <si>
+    <t>Perempuan</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>hahaha</t>
+  </si>
+  <si>
+    <t>TIMEZONE</t>
+  </si>
+  <si>
+    <t>WITA</t>
+  </si>
+  <si>
+    <t>gg1</t>
+  </si>
+  <si>
+    <t>gg2</t>
+  </si>
+  <si>
+    <t>gg3</t>
   </si>
 </sst>
 </file>
@@ -403,7 +433,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="J2" sqref="A1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -457,11 +487,45 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1"/>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
+      <c r="A2" s="2">
+        <v>4223532</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>52534</v>
+      </c>
       <c r="E2" s="3"/>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
change excell value for employee import
</commit_message>
<xml_diff>
--- a/public/assets/EmployeeDcImport.xlsx
+++ b/public/assets/EmployeeDcImport.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>NIK</t>
   </si>
@@ -64,6 +64,9 @@
     <t>PASSWORD</t>
   </si>
   <si>
+    <t>1112</t>
+  </si>
+  <si>
     <t>Demo Cookings</t>
   </si>
   <si>
@@ -76,9 +79,15 @@
     <t>WIB</t>
   </si>
   <si>
+    <t>9812892189</t>
+  </si>
+  <si>
     <t>BTN</t>
   </si>
   <si>
+    <t>2018-11-23</t>
+  </si>
+  <si>
     <t>Agency Name</t>
   </si>
   <si>
@@ -92,6 +101,9 @@
   </si>
   <si>
     <t>Perempuan</t>
+  </si>
+  <si>
+    <t>2018-01-01</t>
   </si>
   <si>
     <t>SD</t>
@@ -104,9 +116,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-  </numFmts>
   <fonts count="4">
     <font>
       <sz val="10.0"/>
@@ -148,14 +157,14 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf quotePrefix="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf quotePrefix="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -233,56 +242,56 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3">
-        <v>1112.0</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="C2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="3">
+        <v>19</v>
+      </c>
+      <c r="D2" s="4">
         <v>2.177180713E9</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="4">
-        <v>9.812892189E9</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="5">
-        <v>43427.0</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="G2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="J2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="K2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="5">
-        <v>43101.0</v>
-      </c>
-      <c r="P2" s="3" t="s">
+      <c r="L2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="M2" s="4" t="s">
         <v>28</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjust import employee mtc, gtc, dc
</commit_message>
<xml_diff>
--- a/public/assets/EmployeeDcImport.xlsx
+++ b/public/assets/EmployeeDcImport.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>NIK</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>1312312312312313</t>
+  </si>
+  <si>
+    <t>02177180713</t>
   </si>
   <si>
     <t>sadas@gmail.com</t>
@@ -251,47 +254,47 @@
       <c r="C2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="4">
-        <v>2.177180713E9</v>
+      <c r="D2" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>